<commit_message>
document update and model2 update
</commit_message>
<xml_diff>
--- a/project_1/3. 요구사항 명세서, 분석서/2조_DLT 요구사항 명세서_v0.1.xlsx
+++ b/project_1/3. 요구사항 명세서, 분석서/2조_DLT 요구사항 명세서_v0.1.xlsx
@@ -595,10 +595,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>사용자의 성별을 체크팍스를 이용하여 입력할 수 있도록 하고 버튼을 눌러 데이터를 제공</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자의 흡연 여부을 체크박스를 이용하여 입력할 수 있도록 하고 버튼을 눌러 데이터를 제공</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1394,6 +1390,10 @@
   </si>
   <si>
     <t>기대 수명 예측(지역별)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자의 성별을 체크박스를 이용하여 입력할 수 있도록 하고 버튼을 눌러 데이터를 제공</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2054,8 +2054,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>6</v>
@@ -2099,21 +2099,21 @@
         <v>5</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>275</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -2184,7 +2184,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>9</v>
@@ -2198,7 +2198,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>12</v>
@@ -2212,7 +2212,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>18</v>
@@ -2226,7 +2226,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>19</v>
@@ -2240,7 +2240,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>14</v>
@@ -2254,7 +2254,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>22</v>
@@ -2268,7 +2268,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>24</v>
@@ -2282,7 +2282,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>25</v>
@@ -2296,7 +2296,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>26</v>
@@ -2311,7 +2311,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>13</v>
@@ -2332,13 +2332,13 @@
         <v>43</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
@@ -2346,105 +2346,105 @@
         <v>158</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>159</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="30" t="s">
         <v>156</v>
@@ -2455,13 +2455,13 @@
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D32" s="31" t="s">
         <v>155</v>
@@ -2469,13 +2469,13 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>21</v>
@@ -2483,24 +2483,24 @@
     </row>
     <row r="34" spans="1:4" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>156</v>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D36" s="31" t="s">
         <v>155</v>
@@ -2525,16 +2525,16 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="31" t="s">
         <v>195</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -2900,178 +2900,178 @@
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B67" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="C67" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="C67" s="24" t="s">
-        <v>224</v>
-      </c>
       <c r="D67" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="B68" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>226</v>
-      </c>
       <c r="D68" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C69" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" s="25" t="s">
         <v>233</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C70" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="B70" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>232</v>
-      </c>
       <c r="D70" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B73" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C73" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="C73" s="24" t="s">
-        <v>241</v>
-      </c>
       <c r="D73" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B75" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="B75" s="24" t="s">
-        <v>240</v>
-      </c>
       <c r="C75" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D75" s="25" t="s">
         <v>252</v>
-      </c>
-      <c r="D75" s="25" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="B78" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="C78" s="24" t="s">
+      <c r="D78" s="25" t="s">
         <v>257</v>
-      </c>
-      <c r="D78" s="25" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C79" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="D79" s="25" t="s">
         <v>259</v>
-      </c>
-      <c r="D79" s="25" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C81" s="16" t="s">
         <v>122</v>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C82" s="16" t="s">
         <v>124</v>
@@ -3096,10 +3096,10 @@
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C83" s="16" t="s">
         <v>126</v>
@@ -3110,10 +3110,10 @@
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C84" s="16" t="s">
         <v>128</v>
@@ -3124,24 +3124,24 @@
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C85" s="16" t="s">
         <v>130</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C86" s="16" t="s">
         <v>131</v>
@@ -3152,10 +3152,10 @@
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>133</v>
@@ -3166,16 +3166,16 @@
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>135</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3186,7 +3186,7 @@
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>136</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B91" s="18" t="s">
         <v>136</v>
@@ -3209,12 +3209,12 @@
         <v>139</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B92" s="18" t="s">
         <v>136</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>136</v>
@@ -3237,12 +3237,12 @@
         <v>135</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B94" s="18" t="s">
         <v>136</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B96" s="21" t="s">
         <v>144</v>
@@ -3265,12 +3265,12 @@
         <v>145</v>
       </c>
       <c r="D96" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B97" s="21" t="s">
         <v>144</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B98" s="21" t="s">
         <v>144</v>
@@ -3293,40 +3293,40 @@
         <v>148</v>
       </c>
       <c r="D98" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B99" s="24" t="s">
         <v>144</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B100" s="24" t="s">
         <v>144</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B102" s="23" t="s">
         <v>149</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="103" spans="1:4" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B103" s="23" t="s">
         <v>149</v>
@@ -3349,12 +3349,12 @@
         <v>139</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B104" s="23" t="s">
         <v>149</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="105" spans="1:4" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B105" s="23" t="s">
         <v>149</v>
@@ -3377,12 +3377,12 @@
         <v>148</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B106" s="23" t="s">
         <v>149</v>
@@ -3396,7 +3396,7 @@
     </row>
     <row r="107" spans="1:4" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A107" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B107" s="23" t="s">
         <v>149</v>

</xml_diff>